<commit_message>
Pandas versioning (closes #31 - #71)
relevant changes:
- enhancing the compatibility with the latest pandas, and xlsxwriter
  versions
- imrpoving the readability and performance of the add_Sectors function
  + unittests
- adding new functionalities to the code to build database templates
  from tabular data (issue #71)
</commit_message>
<xml_diff>
--- a/mario/test/SUT.xlsx
+++ b/mario/test/SUT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10421550_polimi_it/Documents/Politecnico di Milano/Research/Codes/MARIO_tests/tests_database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammadamintahavori/Documents/GitHub/MARIO/mario/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_4248B74F6988705E4743A855A9CA8A1348500252" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE06FF22-2853-4FB2-A169-1CC5CC65CC8A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CD669F-31C3-C941-B900-D91CB5297DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flows" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="20">
   <si>
     <t>RoW</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>Satellite account</t>
-  </si>
-  <si>
-    <t>None</t>
   </si>
   <si>
     <t>Consumption category</t>
@@ -159,7 +156,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -175,9 +172,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -215,9 +212,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -250,26 +247,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -302,26 +282,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -497,41 +460,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="18" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="30.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
@@ -611,7 +574,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
@@ -685,13 +648,13 @@
         <v>9</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
@@ -765,13 +728,13 @@
         <v>7</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -860,7 +823,7 @@
         <v>10593709264.209579</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -949,7 +912,7 @@
         <v>49576189.163435943</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1038,7 +1001,7 @@
         <v>125225295098.9211</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1127,7 +1090,7 @@
         <v>40982970399.814873</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1216,7 +1179,7 @@
         <v>837449917.49965286</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1305,7 +1268,7 @@
         <v>8386754301.1431227</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1394,7 +1357,7 @@
         <v>27866578789.311008</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1483,7 +1446,7 @@
         <v>310096421.82128233</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1572,7 +1535,7 @@
         <v>317067144419.63702</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -1661,7 +1624,7 @@
         <v>1030415406539.422</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -1750,7 +1713,7 @@
         <v>149984734571.46329</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -1839,7 +1802,7 @@
         <v>58616559650.868736</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -1928,7 +1891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -2017,7 +1980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -2106,7 +2069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -2195,7 +2158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -2284,7 +2247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -2373,7 +2336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
@@ -2462,7 +2425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
@@ -2551,7 +2514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
@@ -2640,7 +2603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>8</v>
       </c>
@@ -2729,7 +2692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>8</v>
       </c>
@@ -2818,7 +2781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
@@ -2907,7 +2870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
@@ -2996,7 +2959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>10</v>
       </c>
@@ -3085,7 +3048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
@@ -3174,7 +3137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>10</v>
       </c>
@@ -3182,7 +3145,7 @@
         <v>15</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D31" s="2">
         <v>0</v>
@@ -3272,16 +3235,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -3289,10 +3254,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -3300,10 +3265,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -3311,10 +3276,10 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -3322,10 +3287,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -3333,10 +3298,10 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -3344,10 +3309,10 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -3355,10 +3320,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -3366,10 +3331,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -3377,10 +3342,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -3388,10 +3353,10 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -3399,10 +3364,10 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
@@ -3410,10 +3375,10 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -3421,10 +3386,10 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -3432,10 +3397,10 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -3443,18 +3408,18 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed test SUT file to avoid nan
</commit_message>
<xml_diff>
--- a/mario/test/SUT.xlsx
+++ b/mario/test/SUT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammadamintahavori/Documents/GitHub/MARIO/mario/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzorinaldi/Documents/GitHub/MARIO/mario/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CD669F-31C3-C941-B900-D91CB5297DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B74DC7-545D-4842-B858-4597150132E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4340" yWindow="760" windowWidth="24460" windowHeight="16360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flows" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="21">
   <si>
     <t>RoW</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>M EUR</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -460,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC31"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3145,7 +3148,7 @@
         <v>15</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D31" s="2">
         <v>0</v>
@@ -3235,8 +3238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3416,10 +3419,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>